<commit_message>
Adjusted Resistor Null Offset and Digit Display
</commit_message>
<xml_diff>
--- a/DMM Collected Spreadsheets.xlsx
+++ b/DMM Collected Spreadsheets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Dropbox (Personal)\BannerPrintFiles\Arduino\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\Micro-DMM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715A6BCB-DB71-434D-8A2C-B6E22B4CB5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDF1CFF-DA86-4BA3-80F0-F4E4869FDDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="25580" windowHeight="15260" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
+    <workbookView xWindow="31700" yWindow="-3810" windowWidth="27120" windowHeight="19590" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Analog Circuits Reference" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="262">
   <si>
     <t>DMM Calibration Template</t>
   </si>
@@ -822,6 +822,9 @@
   </si>
   <si>
     <t>V across Sense</t>
+  </si>
+  <si>
+    <t>Approx V Scale Factor</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1017,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="170" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1057,8 +1060,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1069,50 +1108,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1169,9 +1164,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1232,6 +1224,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2315,21 +2310,21 @@
   </sortState>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{8CAD429C-36CF-498D-849C-0098ABC75B14}" name="Reference"/>
-    <tableColumn id="2" xr3:uid="{3C383277-BB03-4B26-B59D-271900A735A1}" name="Value" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{3C383277-BB03-4B26-B59D-271900A735A1}" name="Value" dataDxfId="8"/>
     <tableColumn id="14" xr3:uid="{CAAC0085-7017-44AA-889F-0E7E133EA370}" name="Original"/>
     <tableColumn id="3" xr3:uid="{A6C4183F-E75A-4F46-A769-E53158F7359F}" name="Datasheet"/>
     <tableColumn id="4" xr3:uid="{31A095E3-5BAC-44AF-97E9-A3A12486DC0F}" name="Footprint"/>
     <tableColumn id="5" xr3:uid="{647E944E-F081-491C-98C8-2D51872ADDA4}" name="Qty"/>
     <tableColumn id="6" xr3:uid="{344C4C17-3DB6-42D6-8CE5-9610FEABE750}" name="DNP"/>
-    <tableColumn id="7" xr3:uid="{2B35823C-0E02-441E-BB51-3B294540CD99}" name="Description" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{9C8BB37C-C19E-4E26-9F8E-90B9F913B7AD}" name="Function" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{2B35823C-0E02-441E-BB51-3B294540CD99}" name="Description" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{9C8BB37C-C19E-4E26-9F8E-90B9F913B7AD}" name="Function" dataDxfId="6"/>
     <tableColumn id="9" xr3:uid="{775B051F-40A1-4EF8-947C-8B73B649F287}" name="Purchase Link"/>
-    <tableColumn id="10" xr3:uid="{B9BBEBB7-78B1-46DB-8422-ED127E3B15E2}" name="Cost " dataDxfId="6" dataCellStyle="Currency"/>
+    <tableColumn id="10" xr3:uid="{B9BBEBB7-78B1-46DB-8422-ED127E3B15E2}" name="Cost " dataDxfId="5" dataCellStyle="Currency"/>
     <tableColumn id="11" xr3:uid="{38477E8E-9034-4597-8EB9-23EE541B3E96}" name="Qty2"/>
-    <tableColumn id="12" xr3:uid="{161B492C-27E0-41C6-8A4B-F71EC65AAC28}" name="Cost each" dataDxfId="5" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{161B492C-27E0-41C6-8A4B-F71EC65AAC28}" name="Cost each" dataDxfId="4" dataCellStyle="Currency">
       <calculatedColumnFormula>K3/L3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{86FE0A09-CD2A-4CEF-A252-4872B68E7831}" name="Cost / DMM" dataDxfId="4" dataCellStyle="Currency">
+    <tableColumn id="13" xr3:uid="{86FE0A09-CD2A-4CEF-A252-4872B68E7831}" name="Cost / DMM" dataDxfId="3" dataCellStyle="Currency">
       <calculatedColumnFormula>M3*F3</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{8C8B0D17-5597-4557-93A5-0A15D8997CE9}" name="QTY On Hand" dataDxfId="2" dataCellStyle="Currency"/>
@@ -2661,7 +2656,7 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2684,14 +2679,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
       <c r="O1" s="17" t="s">
         <v>34</v>
       </c>
@@ -3758,7 +3753,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B50" s="15" t="s">
         <v>259</v>
       </c>
@@ -3781,7 +3776,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B51" s="15">
         <v>50</v>
       </c>
@@ -3794,7 +3789,6 @@
         <v>26.053639846743295</v>
       </c>
       <c r="E51" s="15">
-        <f>E48</f>
         <v>44000</v>
       </c>
       <c r="F51" s="15">
@@ -3809,15 +3803,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.35">
       <c r="G53" s="15" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="J53" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.35">
       <c r="G54" s="15">
         <f>D51-F51</f>
         <v>2.1072796934865892</v>
+      </c>
+      <c r="J54" s="15">
+        <f>(C51+G51)/E51</f>
+        <v>22.727272727272727</v>
       </c>
     </row>
   </sheetData>
@@ -3837,7 +3838,7 @@
   <dimension ref="B2:X23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3855,64 +3856,64 @@
       </c>
     </row>
     <row r="3" spans="2:24" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="39" t="s">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
     </row>
     <row r="4" spans="2:24" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="36" t="s">
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="37"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="36" t="s">
+      <c r="H4" s="47"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="37"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="36" t="s">
+      <c r="K4" s="47"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="37"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="36" t="s">
+      <c r="N4" s="47"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="36" t="s">
+      <c r="Q4" s="47"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="46" t="s">
         <v>249</v>
       </c>
-      <c r="T4" s="37"/>
-      <c r="U4" s="38"/>
-      <c r="V4" s="36" t="s">
+      <c r="T4" s="47"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="46" t="s">
         <v>249</v>
       </c>
-      <c r="W4" s="37"/>
-      <c r="X4" s="38"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="48"/>
     </row>
     <row r="5" spans="2:24" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
@@ -4024,16 +4025,16 @@
         <f>_xlfn.TEXTJOIN("",TRUE,,"CF_",$B6," = ",K6,";")</f>
         <v>CF_A = 1.0339;</v>
       </c>
-      <c r="M6" s="13">
-        <v>0.48799999999999999</v>
+      <c r="M6">
+        <v>0.49759999999999999</v>
       </c>
       <c r="N6">
         <f>ROUND($E6/M6,4)</f>
-        <v>1.0061</v>
+        <v>0.98670000000000002</v>
       </c>
       <c r="O6" s="9" t="str">
         <f>_xlfn.TEXTJOIN("",TRUE,,"CF_",$B6," = ",N6,";")</f>
-        <v>CF_A = 1.0061;</v>
+        <v>CF_A = 0.9867;</v>
       </c>
       <c r="P6">
         <v>0.49959999999999999</v>
@@ -4108,16 +4109,16 @@
         <f t="shared" ref="L7:L20" si="4">_xlfn.TEXTJOIN("",TRUE,,"CF_",$B7," = ",K7,";")</f>
         <v>CF_B = 1.0105;</v>
       </c>
-      <c r="M7" s="13">
-        <v>0.98843999999999999</v>
+      <c r="M7">
+        <v>0.99628000000000005</v>
       </c>
       <c r="N7">
         <f t="shared" ref="N7:N20" si="5">ROUND($E7/M7,4)</f>
-        <v>1.0086999999999999</v>
+        <v>1.0006999999999999</v>
       </c>
       <c r="O7" s="9" t="str">
         <f t="shared" ref="O7:O20" si="6">_xlfn.TEXTJOIN("",TRUE,,"CF_",$B7," = ",N7,";")</f>
-        <v>CF_B = 1.0087;</v>
+        <v>CF_B = 1.0007;</v>
       </c>
       <c r="P7">
         <v>1.00118</v>
@@ -4192,16 +4193,16 @@
         <f t="shared" si="4"/>
         <v>CF_C = 0.9958;</v>
       </c>
-      <c r="M8" s="13">
-        <v>4.6307700000000001</v>
+      <c r="M8">
+        <v>4.657</v>
       </c>
       <c r="N8">
         <f t="shared" si="5"/>
-        <v>1.0044</v>
+        <v>0.99870000000000003</v>
       </c>
       <c r="O8" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>CF_C = 1.0044;</v>
+        <v>CF_C = 0.9987;</v>
       </c>
       <c r="P8">
         <v>4.65158</v>
@@ -4276,16 +4277,16 @@
         <f t="shared" si="4"/>
         <v>CF_D = 0.9874;</v>
       </c>
-      <c r="M9" s="13">
-        <v>10.0025</v>
+      <c r="M9">
+        <v>10.050000000000001</v>
       </c>
       <c r="N9">
         <f t="shared" si="5"/>
-        <v>1.0018</v>
+        <v>0.99709999999999999</v>
       </c>
       <c r="O9" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>CF_D = 1.0018;</v>
+        <v>CF_D = 0.9971;</v>
       </c>
       <c r="P9">
         <v>10.0425</v>
@@ -4360,16 +4361,16 @@
         <f t="shared" si="4"/>
         <v>CF_E = 0.9668;</v>
       </c>
-      <c r="M10" s="13">
-        <v>32.620100000000001</v>
+      <c r="M10">
+        <v>33.07</v>
       </c>
       <c r="N10">
         <f t="shared" si="5"/>
-        <v>1.0088999999999999</v>
+        <v>0.99519999999999997</v>
       </c>
       <c r="O10" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>CF_E = 1.0089;</v>
+        <v>CF_E = 0.9952;</v>
       </c>
       <c r="P10">
         <v>33.062600000000003</v>
@@ -4444,16 +4445,16 @@
         <f t="shared" si="4"/>
         <v>CF_F = 1.0131;</v>
       </c>
-      <c r="M11" s="13">
-        <v>97.731999999999999</v>
+      <c r="M11">
+        <v>99.88</v>
       </c>
       <c r="N11">
         <f t="shared" si="5"/>
-        <v>1.018</v>
+        <v>0.99609999999999999</v>
       </c>
       <c r="O11" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>CF_F = 1.018;</v>
+        <v>CF_F = 0.9961;</v>
       </c>
       <c r="P11">
         <v>99.843900000000005</v>
@@ -4528,16 +4529,16 @@
         <f t="shared" si="4"/>
         <v>CF_G = 1.0043;</v>
       </c>
-      <c r="M12" s="13">
-        <v>328.89</v>
+      <c r="M12">
+        <v>332.5</v>
       </c>
       <c r="N12">
         <f t="shared" si="5"/>
-        <v>1.0079</v>
+        <v>0.997</v>
       </c>
       <c r="O12" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>CF_G = 1.0079;</v>
+        <v>CF_G = 0.997;</v>
       </c>
       <c r="P12">
         <v>332.18</v>
@@ -4612,16 +4613,16 @@
         <f t="shared" si="4"/>
         <v>CF_H = 1.0003;</v>
       </c>
-      <c r="M13" s="13">
-        <v>995.08579999999995</v>
+      <c r="M13">
+        <v>995.67759999999998</v>
       </c>
       <c r="N13">
         <f t="shared" si="5"/>
-        <v>1.0049999999999999</v>
+        <v>1.0044</v>
       </c>
       <c r="O13" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>CF_H = 1.005;</v>
+        <v>CF_H = 1.0044;</v>
       </c>
       <c r="P13">
         <v>996.72630000000004</v>
@@ -4696,16 +4697,16 @@
         <f t="shared" si="4"/>
         <v>CF_I = 0.9991;</v>
       </c>
-      <c r="M14" s="13">
-        <v>2992.9265</v>
+      <c r="M14">
+        <v>2992.8353999999999</v>
       </c>
       <c r="N14">
         <f t="shared" si="5"/>
-        <v>1.0029999999999999</v>
+        <v>1.0031000000000001</v>
       </c>
       <c r="O14" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>CF_I = 1.003;</v>
+        <v>CF_I = 1.0031;</v>
       </c>
       <c r="P14">
         <v>2995.6271999999999</v>
@@ -4780,16 +4781,16 @@
         <f t="shared" si="4"/>
         <v>CF_J = 0.9983;</v>
       </c>
-      <c r="M15" s="13">
-        <v>9884.3086000000003</v>
+      <c r="M15">
+        <v>9905.3516</v>
       </c>
       <c r="N15">
         <f t="shared" si="5"/>
-        <v>1.0044</v>
+        <v>1.0023</v>
       </c>
       <c r="O15" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>CF_J = 1.0044;</v>
+        <v>CF_J = 1.0023;</v>
       </c>
       <c r="P15">
         <v>9916.1718999999994</v>
@@ -4864,16 +4865,16 @@
         <f t="shared" si="4"/>
         <v>CF_K = 0.999;</v>
       </c>
-      <c r="M16" s="13">
-        <v>32739.656200000001</v>
+      <c r="M16">
+        <v>32825.832000000002</v>
       </c>
       <c r="N16">
         <f t="shared" si="5"/>
-        <v>1.0069999999999999</v>
+        <v>1.0044</v>
       </c>
       <c r="O16" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>CF_K = 1.007;</v>
+        <v>CF_K = 1.0044;</v>
       </c>
       <c r="P16">
         <v>32868.027300000002</v>
@@ -4948,16 +4949,16 @@
         <f t="shared" si="4"/>
         <v>CF_L = 0.9969;</v>
       </c>
-      <c r="M17" s="13">
-        <v>98448.616999999998</v>
+      <c r="M17">
+        <v>99177.039000000004</v>
       </c>
       <c r="N17">
         <f t="shared" si="5"/>
-        <v>1.0166999999999999</v>
+        <v>1.0092000000000001</v>
       </c>
       <c r="O17" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>CF_L = 1.0167;</v>
+        <v>CF_L = 1.0092;</v>
       </c>
       <c r="P17">
         <v>99363.991999999998</v>
@@ -5032,16 +5033,16 @@
         <f t="shared" si="4"/>
         <v>CF_M = 0.9956;</v>
       </c>
-      <c r="M18" s="13">
-        <v>311396.18800000002</v>
+      <c r="M18">
+        <v>319441.65600000002</v>
       </c>
       <c r="N18">
         <f t="shared" si="5"/>
-        <v>1.0482</v>
+        <v>1.0218</v>
       </c>
       <c r="O18" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>CF_M = 1.0482;</v>
+        <v>CF_M = 1.0218;</v>
       </c>
       <c r="P18">
         <v>320741.84399999998</v>
@@ -5116,16 +5117,16 @@
         <f t="shared" si="4"/>
         <v>CF_N = 0.9627;</v>
       </c>
-      <c r="M19" s="13">
-        <v>917167</v>
+      <c r="M19">
+        <v>968296.4375</v>
       </c>
       <c r="N19">
         <f t="shared" si="5"/>
-        <v>1.1323000000000001</v>
+        <v>1.0725</v>
       </c>
       <c r="O19" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>CF_N = 1.1323;</v>
+        <v>CF_N = 1.0725;</v>
       </c>
       <c r="P19">
         <v>978735.125</v>
@@ -5200,16 +5201,16 @@
         <f t="shared" si="4"/>
         <v>CF_O = 0.6932;</v>
       </c>
-      <c r="M20" s="14">
-        <v>3054930.5</v>
+      <c r="M20">
+        <v>3834936.25</v>
       </c>
       <c r="N20" s="11">
         <f t="shared" si="5"/>
-        <v>1.5401</v>
+        <v>1.2269000000000001</v>
       </c>
       <c r="O20" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>CF_O = 1.5401;</v>
+        <v>CF_O = 1.2269;</v>
       </c>
       <c r="P20">
         <v>4227492</v>
@@ -5246,36 +5247,36 @@
       </c>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="G21" s="33" t="s">
+      <c r="G21" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="34"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="33" t="s">
+      <c r="H21" s="50"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="K21" s="34"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="33" t="s">
+      <c r="K21" s="50"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="N21" s="34"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="33" t="s">
+      <c r="N21" s="50"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="35"/>
-      <c r="S21" s="33" t="s">
+      <c r="Q21" s="50"/>
+      <c r="R21" s="51"/>
+      <c r="S21" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="T21" s="34"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="33" t="s">
+      <c r="T21" s="50"/>
+      <c r="U21" s="51"/>
+      <c r="V21" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="W21" s="34"/>
-      <c r="X21" s="35"/>
+      <c r="W21" s="50"/>
+      <c r="X21" s="51"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.35">
       <c r="G22" s="13" t="s">
@@ -5486,7 +5487,7 @@
       <c r="A3" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="39" t="s">
         <v>78</v>
       </c>
       <c r="C3" t="s">
@@ -5517,17 +5518,17 @@
         <v>100</v>
       </c>
       <c r="M3" s="27">
-        <f t="shared" ref="M3:M39" si="0">K3/L3</f>
+        <f t="shared" ref="M3:M36" si="0">K3/L3</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="N3" s="27">
-        <f t="shared" ref="N3:N39" si="1">M3*F3</f>
+        <f t="shared" ref="N3:N36" si="1">M3*F3</f>
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="O3" s="55">
+      <c r="O3" s="42">
         <v>10</v>
       </c>
-      <c r="P3" s="55">
+      <c r="P3" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>10</v>
       </c>
@@ -5536,7 +5537,7 @@
       <c r="A4" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="39" t="s">
         <v>87</v>
       </c>
       <c r="C4" t="s">
@@ -5574,10 +5575,10 @@
         <f t="shared" si="1"/>
         <v>0.16600000000000001</v>
       </c>
-      <c r="O4" s="55">
+      <c r="O4" s="42">
         <v>19</v>
       </c>
-      <c r="P4" s="55">
+      <c r="P4" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>9</v>
       </c>
@@ -5586,7 +5587,7 @@
       <c r="A5" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="39" t="s">
         <v>90</v>
       </c>
       <c r="C5" t="s">
@@ -5624,10 +5625,10 @@
         <f t="shared" si="1"/>
         <v>1.6E-2</v>
       </c>
-      <c r="O5" s="55">
+      <c r="O5" s="42">
         <v>100</v>
       </c>
-      <c r="P5" s="55">
+      <c r="P5" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>100</v>
       </c>
@@ -5636,7 +5637,7 @@
       <c r="A6" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="39" t="s">
         <v>83</v>
       </c>
       <c r="C6" t="s">
@@ -5674,10 +5675,10 @@
         <f t="shared" si="1"/>
         <v>0.12400000000000001</v>
       </c>
-      <c r="O6" s="55">
+      <c r="O6" s="42">
         <v>20</v>
       </c>
-      <c r="P6" s="55">
+      <c r="P6" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>10</v>
       </c>
@@ -5686,7 +5687,7 @@
       <c r="A7" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="39" t="s">
         <v>85</v>
       </c>
       <c r="C7" t="s">
@@ -5724,10 +5725,10 @@
         <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
-      <c r="O7" s="55">
+      <c r="O7" s="42">
         <v>0</v>
       </c>
-      <c r="P7" s="55">
+      <c r="P7" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>0</v>
       </c>
@@ -5736,7 +5737,7 @@
       <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="39" t="s">
         <v>86</v>
       </c>
       <c r="C8" t="s">
@@ -5774,10 +5775,10 @@
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="O8" s="55">
+      <c r="O8" s="42">
         <v>15</v>
       </c>
-      <c r="P8" s="55">
+      <c r="P8" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>5</v>
       </c>
@@ -5786,7 +5787,7 @@
       <c r="A9" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="39" t="s">
         <v>63</v>
       </c>
       <c r="C9" t="s">
@@ -5824,10 +5825,10 @@
         <f t="shared" si="1"/>
         <v>0.14299999999999999</v>
       </c>
-      <c r="O9" s="55">
+      <c r="O9" s="42">
         <v>15</v>
       </c>
-      <c r="P9" s="55">
+      <c r="P9" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>15</v>
       </c>
@@ -5836,7 +5837,7 @@
       <c r="A10" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="39" t="s">
         <v>94</v>
       </c>
       <c r="C10" t="s">
@@ -5874,10 +5875,10 @@
         <f t="shared" si="1"/>
         <v>0.40800000000000003</v>
       </c>
-      <c r="O10" s="55">
+      <c r="O10" s="42">
         <v>90</v>
       </c>
-      <c r="P10" s="55">
+      <c r="P10" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>45</v>
       </c>
@@ -5886,7 +5887,7 @@
       <c r="A11" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="39" t="s">
         <v>98</v>
       </c>
       <c r="C11" t="s">
@@ -5924,8 +5925,8 @@
         <f t="shared" si="1"/>
         <v>0.1898</v>
       </c>
-      <c r="O11" s="55"/>
-      <c r="P11" s="55">
+      <c r="O11" s="42"/>
+      <c r="P11" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>0</v>
       </c>
@@ -5934,7 +5935,7 @@
       <c r="A12" t="s">
         <v>109</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="39" t="s">
         <v>110</v>
       </c>
       <c r="C12" t="s">
@@ -5969,8 +5970,8 @@
         <f t="shared" si="1"/>
         <v>0.13980000000000001</v>
       </c>
-      <c r="O12" s="55"/>
-      <c r="P12" s="55">
+      <c r="O12" s="42"/>
+      <c r="P12" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>0</v>
       </c>
@@ -5979,7 +5980,7 @@
       <c r="A13" t="s">
         <v>112</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="39" t="s">
         <v>113</v>
       </c>
       <c r="C13" t="s">
@@ -6014,8 +6015,8 @@
         <f t="shared" si="1"/>
         <v>0.13980000000000001</v>
       </c>
-      <c r="O13" s="55"/>
-      <c r="P13" s="55">
+      <c r="O13" s="42"/>
+      <c r="P13" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>0</v>
       </c>
@@ -6024,7 +6025,7 @@
       <c r="A14" t="s">
         <v>116</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="39" t="s">
         <v>117</v>
       </c>
       <c r="C14" t="s">
@@ -6059,8 +6060,8 @@
         <f t="shared" si="1"/>
         <v>1.798</v>
       </c>
-      <c r="O14" s="55"/>
-      <c r="P14" s="55">
+      <c r="O14" s="42"/>
+      <c r="P14" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>0</v>
       </c>
@@ -6069,7 +6070,7 @@
       <c r="A15" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="39" t="s">
         <v>102</v>
       </c>
       <c r="C15" t="s">
@@ -6104,8 +6105,8 @@
         <f t="shared" si="1"/>
         <v>0.13980000000000001</v>
       </c>
-      <c r="O15" s="55"/>
-      <c r="P15" s="55">
+      <c r="O15" s="42"/>
+      <c r="P15" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>0</v>
       </c>
@@ -6114,7 +6115,7 @@
       <c r="A16" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="39" t="s">
         <v>106</v>
       </c>
       <c r="C16" t="s">
@@ -6149,8 +6150,8 @@
         <f t="shared" si="1"/>
         <v>0.13980000000000001</v>
       </c>
-      <c r="O16" s="55"/>
-      <c r="P16" s="55">
+      <c r="O16" s="42"/>
+      <c r="P16" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>0</v>
       </c>
@@ -6159,7 +6160,7 @@
       <c r="A17" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="39" t="s">
         <v>120</v>
       </c>
       <c r="C17" t="s">
@@ -6194,10 +6195,10 @@
         <f t="shared" si="1"/>
         <v>0.20400000000000001</v>
       </c>
-      <c r="O17" s="55">
+      <c r="O17" s="42">
         <v>13</v>
       </c>
-      <c r="P17" s="55">
+      <c r="P17" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>13</v>
       </c>
@@ -6206,7 +6207,7 @@
       <c r="A18" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="39" t="s">
         <v>124</v>
       </c>
       <c r="C18" t="s">
@@ -6244,10 +6245,10 @@
         <f t="shared" si="1"/>
         <v>0.15920000000000001</v>
       </c>
-      <c r="O18" s="55">
+      <c r="O18" s="42">
         <v>20</v>
       </c>
-      <c r="P18" s="55">
+      <c r="P18" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>5</v>
       </c>
@@ -6256,7 +6257,7 @@
       <c r="A19" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="39" t="s">
         <v>128</v>
       </c>
       <c r="C19" t="s">
@@ -6294,10 +6295,10 @@
         <f t="shared" si="1"/>
         <v>0.20699999999999999</v>
       </c>
-      <c r="O19" s="55">
+      <c r="O19" s="42">
         <v>16</v>
       </c>
-      <c r="P19" s="55">
+      <c r="P19" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>16</v>
       </c>
@@ -6306,7 +6307,7 @@
       <c r="A20" t="s">
         <v>132</v>
       </c>
-      <c r="B20" s="51">
+      <c r="B20" s="39">
         <v>500</v>
       </c>
       <c r="C20" t="s">
@@ -6344,10 +6345,10 @@
         <f t="shared" si="1"/>
         <v>1.1200000000000002E-2</v>
       </c>
-      <c r="O20" s="55">
+      <c r="O20" s="42">
         <v>10</v>
       </c>
-      <c r="P20" s="55">
+      <c r="P20" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>10</v>
       </c>
@@ -6356,7 +6357,7 @@
       <c r="A21" t="s">
         <v>141</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="39" t="s">
         <v>225</v>
       </c>
       <c r="C21" t="s">
@@ -6394,8 +6395,8 @@
         <f t="shared" si="1"/>
         <v>8.199999999999999E-3</v>
       </c>
-      <c r="O21" s="55"/>
-      <c r="P21" s="55">
+      <c r="O21" s="42"/>
+      <c r="P21" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>0</v>
       </c>
@@ -6404,7 +6405,7 @@
       <c r="A22" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="39" t="s">
         <v>143</v>
       </c>
       <c r="C22" t="s">
@@ -6442,10 +6443,10 @@
         <f t="shared" si="1"/>
         <v>0.186</v>
       </c>
-      <c r="O22" s="55">
+      <c r="O22" s="42">
         <v>4</v>
       </c>
-      <c r="P22" s="55">
+      <c r="P22" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>2</v>
       </c>
@@ -6454,7 +6455,7 @@
       <c r="A23" t="s">
         <v>136</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="39" t="s">
         <v>137</v>
       </c>
       <c r="C23" t="s">
@@ -6492,10 +6493,10 @@
         <f t="shared" si="1"/>
         <v>0.1608</v>
       </c>
-      <c r="O23" s="55">
+      <c r="O23" s="42">
         <v>50</v>
       </c>
-      <c r="P23" s="55">
+      <c r="P23" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>8</v>
       </c>
@@ -6504,7 +6505,7 @@
       <c r="A24" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="51">
+      <c r="B24" s="39">
         <v>62</v>
       </c>
       <c r="C24" t="s">
@@ -6542,10 +6543,10 @@
         <f t="shared" si="1"/>
         <v>0.1386</v>
       </c>
-      <c r="O24" s="55">
+      <c r="O24" s="42">
         <v>40</v>
       </c>
-      <c r="P24" s="55">
+      <c r="P24" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>40</v>
       </c>
@@ -6554,7 +6555,7 @@
       <c r="A25" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="51">
+      <c r="B25" s="39">
         <v>330</v>
       </c>
       <c r="C25" t="s">
@@ -6592,10 +6593,10 @@
         <f t="shared" si="1"/>
         <v>3.9E-2</v>
       </c>
-      <c r="O25" s="55">
+      <c r="O25" s="42">
         <v>30</v>
       </c>
-      <c r="P25" s="55">
+      <c r="P25" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>30</v>
       </c>
@@ -6604,7 +6605,7 @@
       <c r="A26" t="s">
         <v>223</v>
       </c>
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="39" t="s">
         <v>221</v>
       </c>
       <c r="C26" t="s">
@@ -6642,8 +6643,8 @@
         <f t="shared" si="1"/>
         <v>1.8299999999999997E-2</v>
       </c>
-      <c r="O26" s="55"/>
-      <c r="P26" s="55">
+      <c r="O26" s="42"/>
+      <c r="P26" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>0</v>
       </c>
@@ -6652,7 +6653,7 @@
       <c r="A27" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="39" t="s">
         <v>140</v>
       </c>
       <c r="C27" t="s">
@@ -6690,10 +6691,10 @@
         <f t="shared" si="1"/>
         <v>7.8799999999999995E-2</v>
       </c>
-      <c r="O27" s="55">
+      <c r="O27" s="42">
         <v>70</v>
       </c>
-      <c r="P27" s="55">
+      <c r="P27" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>35</v>
       </c>
@@ -6702,7 +6703,7 @@
       <c r="A28" t="s">
         <v>191</v>
       </c>
-      <c r="B28" s="51"/>
+      <c r="B28" s="39"/>
       <c r="C28" t="s">
         <v>17</v>
       </c>
@@ -6732,8 +6733,8 @@
         <f t="shared" si="1"/>
         <v>9.3200000000000005E-2</v>
       </c>
-      <c r="O28" s="55"/>
-      <c r="P28" s="55">
+      <c r="O28" s="42"/>
+      <c r="P28" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>0</v>
       </c>
@@ -6742,7 +6743,7 @@
       <c r="A29" t="s">
         <v>146</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="39" t="s">
         <v>147</v>
       </c>
       <c r="C29" t="s">
@@ -6780,10 +6781,10 @@
         <f t="shared" si="1"/>
         <v>5.4000000000000006E-2</v>
       </c>
-      <c r="O29" s="55">
+      <c r="O29" s="42">
         <v>6</v>
       </c>
-      <c r="P29" s="55">
+      <c r="P29" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>6</v>
       </c>
@@ -6792,7 +6793,7 @@
       <c r="A30" t="s">
         <v>192</v>
       </c>
-      <c r="B30" s="51" t="s">
+      <c r="B30" s="39" t="s">
         <v>144</v>
       </c>
       <c r="C30" t="s">
@@ -6827,10 +6828,10 @@
         <f t="shared" si="1"/>
         <v>0.48719999999999997</v>
       </c>
-      <c r="O30" s="55">
+      <c r="O30" s="42">
         <v>20</v>
       </c>
-      <c r="P30" s="55">
+      <c r="P30" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>6</v>
       </c>
@@ -6839,7 +6840,7 @@
       <c r="A31" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="51" t="s">
+      <c r="B31" s="39" t="s">
         <v>152</v>
       </c>
       <c r="C31" t="s">
@@ -6874,10 +6875,10 @@
         <f t="shared" si="1"/>
         <v>0.36520000000000002</v>
       </c>
-      <c r="O31" s="55">
+      <c r="O31" s="42">
         <v>5</v>
       </c>
-      <c r="P31" s="55">
+      <c r="P31" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>5</v>
       </c>
@@ -6886,7 +6887,7 @@
       <c r="A32" t="s">
         <v>172</v>
       </c>
-      <c r="B32" s="51" t="s">
+      <c r="B32" s="39" t="s">
         <v>173</v>
       </c>
       <c r="C32" t="s">
@@ -6924,10 +6925,10 @@
         <f t="shared" si="1"/>
         <v>0.47960000000000003</v>
       </c>
-      <c r="O32" s="55">
+      <c r="O32" s="42">
         <v>20</v>
       </c>
-      <c r="P32" s="55">
+      <c r="P32" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>20</v>
       </c>
@@ -6936,7 +6937,7 @@
       <c r="A33" t="s">
         <v>177</v>
       </c>
-      <c r="B33" s="51" t="s">
+      <c r="B33" s="39" t="s">
         <v>178</v>
       </c>
       <c r="C33" t="s">
@@ -6974,10 +6975,10 @@
         <f t="shared" si="1"/>
         <v>0.47960000000000003</v>
       </c>
-      <c r="O33" s="55">
+      <c r="O33" s="42">
         <v>20</v>
       </c>
-      <c r="P33" s="55">
+      <c r="P33" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>20</v>
       </c>
@@ -6986,7 +6987,7 @@
       <c r="A34" t="s">
         <v>156</v>
       </c>
-      <c r="B34" s="51" t="s">
+      <c r="B34" s="39" t="s">
         <v>157</v>
       </c>
       <c r="C34" t="s">
@@ -7021,10 +7022,10 @@
         <f t="shared" si="1"/>
         <v>3.3310000000000004</v>
       </c>
-      <c r="O34" s="55">
+      <c r="O34" s="42">
         <v>1</v>
       </c>
-      <c r="P34" s="55">
+      <c r="P34" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>1</v>
       </c>
@@ -7033,7 +7034,7 @@
       <c r="A35" t="s">
         <v>161</v>
       </c>
-      <c r="B35" s="51" t="s">
+      <c r="B35" s="39" t="s">
         <v>162</v>
       </c>
       <c r="C35" t="s">
@@ -7071,10 +7072,10 @@
         <f t="shared" si="1"/>
         <v>1.85</v>
       </c>
-      <c r="O35" s="55">
+      <c r="O35" s="42">
         <v>2</v>
       </c>
-      <c r="P35" s="55">
+      <c r="P35" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>2</v>
       </c>
@@ -7083,7 +7084,7 @@
       <c r="A36" t="s">
         <v>167</v>
       </c>
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="39" t="s">
         <v>168</v>
       </c>
       <c r="C36" t="s">
@@ -7118,16 +7119,16 @@
         <f t="shared" si="1"/>
         <v>0.27079999999999999</v>
       </c>
-      <c r="O36" s="55">
+      <c r="O36" s="42">
         <v>20</v>
       </c>
-      <c r="P36" s="55">
+      <c r="P36" s="42">
         <f>ROUNDDOWN(Table1[[#This Row],[QTY On Hand]]/Table1[[#This Row],[Qty]],0)</f>
         <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="51"/>
+      <c r="B37" s="39"/>
       <c r="H37" s="5"/>
       <c r="K37" s="27"/>
       <c r="M37" s="27"/>
@@ -7136,14 +7137,14 @@
       <c r="P37" s="27"/>
     </row>
     <row r="38" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="51"/>
+      <c r="B38" s="39"/>
       <c r="H38" s="5"/>
       <c r="K38" s="27"/>
       <c r="M38" s="27"/>
       <c r="N38" s="27"/>
     </row>
     <row r="39" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="51"/>
+      <c r="B39" s="39"/>
       <c r="H39" s="5"/>
       <c r="K39" s="27"/>
       <c r="L39" t="s">
@@ -7158,104 +7159,99 @@
       <c r="A40" s="25" t="s">
         <v>247</v>
       </c>
-      <c r="B40" s="51"/>
+      <c r="B40" s="39"/>
       <c r="H40" s="5"/>
       <c r="K40" s="27"/>
       <c r="M40" s="27"/>
       <c r="N40" s="27"/>
     </row>
     <row r="41" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="41" t="s">
+      <c r="A41" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="40" t="s">
         <v>231</v>
       </c>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41">
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32">
         <v>1</v>
       </c>
-      <c r="G41" s="41"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="44"/>
-      <c r="J41" s="41"/>
-      <c r="K41" s="45">
+      <c r="G41" s="32"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="35">
         <v>12.59</v>
       </c>
-      <c r="L41" s="41">
+      <c r="L41" s="32">
         <v>3</v>
       </c>
-      <c r="M41" s="46">
+      <c r="M41" s="36">
         <f>K41/L41</f>
         <v>4.1966666666666663</v>
       </c>
-      <c r="N41" s="46">
+      <c r="N41" s="36">
         <f>M41*F41</f>
         <v>4.1966666666666663</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="42" t="s">
+      <c r="A42" t="s">
         <v>232</v>
       </c>
-      <c r="B42" s="53"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42">
+      <c r="B42" s="39"/>
+      <c r="F42">
         <v>1</v>
       </c>
-      <c r="G42" s="42"/>
-      <c r="H42" s="47"/>
-      <c r="I42" s="47"/>
-      <c r="J42" s="42" t="s">
+      <c r="H42" s="5"/>
+      <c r="J42" t="s">
         <v>233</v>
       </c>
-      <c r="K42" s="48">
+      <c r="K42" s="27">
         <v>18.989999999999998</v>
       </c>
-      <c r="L42" s="42">
+      <c r="L42">
         <v>4</v>
       </c>
-      <c r="M42" s="48">
+      <c r="M42" s="27">
         <f>K42/L42</f>
         <v>4.7474999999999996</v>
       </c>
-      <c r="N42" s="48">
+      <c r="N42" s="27">
         <f>M42*F42</f>
         <v>4.7474999999999996</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="B43" s="54"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43">
+      <c r="B43" s="41"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33">
         <v>1</v>
       </c>
-      <c r="G43" s="43"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="43" t="s">
+      <c r="G43" s="33"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="K43" s="50">
+      <c r="K43" s="38">
         <v>12.88</v>
       </c>
-      <c r="L43" s="43">
+      <c r="L43" s="33">
         <v>5</v>
       </c>
-      <c r="M43" s="50">
+      <c r="M43" s="38">
         <f>K43/L43</f>
         <v>2.5760000000000001</v>
       </c>
-      <c r="N43" s="50">
+      <c r="N43" s="38">
         <f>M43*F43</f>
         <v>2.5760000000000001</v>
       </c>
@@ -7294,7 +7290,7 @@
         <v>50</v>
       </c>
       <c r="M48" s="30">
-        <f>K48/L48</f>
+        <f t="shared" ref="M48:M53" si="2">K48/L48</f>
         <v>1.84</v>
       </c>
     </row>
@@ -7309,7 +7305,7 @@
         <v>50</v>
       </c>
       <c r="M49" s="30">
-        <f>K49/L49</f>
+        <f t="shared" si="2"/>
         <v>1.5318000000000001</v>
       </c>
     </row>
@@ -7324,7 +7320,7 @@
         <v>50</v>
       </c>
       <c r="M50" s="30">
-        <f>K50/L50</f>
+        <f t="shared" si="2"/>
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -7339,7 +7335,7 @@
         <v>50</v>
       </c>
       <c r="M51" s="30">
-        <f>K51/L51</f>
+        <f t="shared" si="2"/>
         <v>0.24</v>
       </c>
     </row>
@@ -7355,7 +7351,7 @@
         <v>50</v>
       </c>
       <c r="M52" s="30">
-        <f>K52/L52</f>
+        <f t="shared" si="2"/>
         <v>11.520166666666666</v>
       </c>
     </row>
@@ -7371,7 +7367,7 @@
         <v>50</v>
       </c>
       <c r="M53" s="30">
-        <f>K53/L53</f>
+        <f t="shared" si="2"/>
         <v>12.502699999999999</v>
       </c>
     </row>
@@ -7387,7 +7383,7 @@
         <v>50</v>
       </c>
       <c r="M55" s="31">
-        <f t="shared" ref="M55" si="2">SUM(M48:M53)</f>
+        <f t="shared" ref="M55" si="3">SUM(M48:M53)</f>
         <v>29.834666666666664</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Calibrating the Giga Version
1256 Version remains completely non functional
</commit_message>
<xml_diff>
--- a/DMM Collected Spreadsheets.xlsx
+++ b/DMM Collected Spreadsheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\Micro-DMM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDF1CFF-DA86-4BA3-80F0-F4E4869FDDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776E5225-6953-4530-86D1-D04E29F32FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31700" yWindow="-3810" windowWidth="27120" windowHeight="19590" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
+    <workbookView xWindow="1850" yWindow="220" windowWidth="21430" windowHeight="14650" activeTab="1" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Analog Circuits Reference" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="263">
   <si>
     <t>DMM Calibration Template</t>
   </si>
@@ -825,6 +825,9 @@
   </si>
   <si>
     <t>Approx V Scale Factor</t>
+  </si>
+  <si>
+    <t>Giga</t>
   </si>
 </sst>
 </file>
@@ -2655,7 +2658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864BF7E5-8FFC-4F13-8BB7-D25F071FB544}">
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
@@ -3835,10 +3838,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CD8753-48D8-45C9-9873-856BE8983C8C}">
-  <dimension ref="B2:X23"/>
+  <dimension ref="B2:AA29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3850,12 +3853,12 @@
     <col min="7" max="18" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:24" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:27" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="45" t="s">
         <v>29</v>
       </c>
@@ -3878,7 +3881,7 @@
       <c r="Q3" s="44"/>
       <c r="R3" s="44"/>
     </row>
-    <row r="4" spans="2:24" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:27" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="45"/>
       <c r="C4" s="45"/>
       <c r="D4" s="45"/>
@@ -3914,8 +3917,13 @@
       </c>
       <c r="W4" s="47"/>
       <c r="X4" s="48"/>
-    </row>
-    <row r="5" spans="2:24" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="Y4" s="46" t="s">
+        <v>262</v>
+      </c>
+      <c r="Z4" s="47"/>
+      <c r="AA4" s="48"/>
+    </row>
+    <row r="5" spans="2:27" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -3985,8 +3993,17 @@
       <c r="X5" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA5" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -4069,8 +4086,19 @@
         <f>_xlfn.TEXTJOIN("",TRUE,,"CF_",$B6," = ",W6,";")</f>
         <v>CF_A = 0.9759;</v>
       </c>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y6">
+        <v>0.5111</v>
+      </c>
+      <c r="Z6">
+        <f>ROUND($E6/Y6,4)</f>
+        <v>0.9607</v>
+      </c>
+      <c r="AA6" s="9" t="str">
+        <f>_xlfn.TEXTJOIN("",TRUE,,"CF_",$B6," = ",Z6,";")</f>
+        <v>CF_A = 0.9607;</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -4153,8 +4181,19 @@
         <f t="shared" ref="X7:X20" si="12">_xlfn.TEXTJOIN("",TRUE,,"CF_",$B7," = ",W7,";")</f>
         <v>CF_B = 0.9963;</v>
       </c>
-    </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y7">
+        <v>1.0124</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" ref="Z7:Z20" si="13">ROUND($E7/Y7,4)</f>
+        <v>0.98480000000000001</v>
+      </c>
+      <c r="AA7" s="9" t="str">
+        <f t="shared" ref="AA7:AA20" si="14">_xlfn.TEXTJOIN("",TRUE,,"CF_",$B7," = ",Z7,";")</f>
+        <v>CF_B = 0.9848;</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -4237,8 +4276,19 @@
         <f t="shared" si="12"/>
         <v>CF_C = 0.9984;</v>
       </c>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y8">
+        <v>4.6651999999999996</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="13"/>
+        <v>0.997</v>
+      </c>
+      <c r="AA8" s="9" t="str">
+        <f t="shared" si="14"/>
+        <v>CF_C = 0.997;</v>
+      </c>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -4321,8 +4371,19 @@
         <f t="shared" si="12"/>
         <v>CF_D = 0.9973;</v>
       </c>
-    </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y9">
+        <v>10.063000000000001</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="13"/>
+        <v>0.99580000000000002</v>
+      </c>
+      <c r="AA9" s="9" t="str">
+        <f t="shared" si="14"/>
+        <v>CF_D = 0.9958;</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -4405,8 +4466,19 @@
         <f t="shared" si="12"/>
         <v>CF_E = 0.9953;</v>
       </c>
-    </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y10">
+        <v>33.128</v>
+      </c>
+      <c r="Z10" s="24">
+        <f t="shared" si="13"/>
+        <v>0.99339999999999995</v>
+      </c>
+      <c r="AA10" s="9" t="str">
+        <f t="shared" si="14"/>
+        <v>CF_E = 0.9934;</v>
+      </c>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -4489,8 +4561,19 @@
         <f t="shared" si="12"/>
         <v>CF_F = 0.9965;</v>
       </c>
-    </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y11">
+        <v>99.84</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="13"/>
+        <v>0.99650000000000005</v>
+      </c>
+      <c r="AA11" s="9" t="str">
+        <f t="shared" si="14"/>
+        <v>CF_F = 0.9965;</v>
+      </c>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -4573,8 +4656,19 @@
         <f t="shared" si="12"/>
         <v>CF_G = 0.9974;</v>
       </c>
-    </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y12">
+        <v>332.09</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="13"/>
+        <v>0.99819999999999998</v>
+      </c>
+      <c r="AA12" s="9" t="str">
+        <f t="shared" si="14"/>
+        <v>CF_G = 0.9982;</v>
+      </c>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -4657,8 +4751,19 @@
         <f t="shared" si="12"/>
         <v>CF_H = 1.0034;</v>
       </c>
-    </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y13">
+        <v>997.34690000000001</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="13"/>
+        <v>1.0027999999999999</v>
+      </c>
+      <c r="AA13" s="9" t="str">
+        <f t="shared" si="14"/>
+        <v>CF_H = 1.0028;</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -4741,8 +4846,19 @@
         <f t="shared" si="12"/>
         <v>CF_I = 1.0018;</v>
       </c>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y14">
+        <v>2998.3438000000001</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="13"/>
+        <v>1.0012000000000001</v>
+      </c>
+      <c r="AA14" s="9" t="str">
+        <f t="shared" si="14"/>
+        <v>CF_I = 1.0012;</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -4825,8 +4941,19 @@
         <f t="shared" si="12"/>
         <v>CF_J = 1.0023;</v>
       </c>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y15">
+        <v>9923.2988000000005</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="13"/>
+        <v>1.0004999999999999</v>
+      </c>
+      <c r="AA15" s="9" t="str">
+        <f t="shared" si="14"/>
+        <v>CF_J = 1.0005;</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -4909,8 +5036,19 @@
         <f t="shared" si="12"/>
         <v>CF_K = 1.0026;</v>
       </c>
-    </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y16">
+        <v>32913.148399999998</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="13"/>
+        <v>1.0017</v>
+      </c>
+      <c r="AA16" s="9" t="str">
+        <f t="shared" si="14"/>
+        <v>CF_K = 1.0017;</v>
+      </c>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -4993,8 +5131,19 @@
         <f t="shared" si="12"/>
         <v>CF_L = 1.0063;</v>
       </c>
-    </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y17">
+        <v>99742.68</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="13"/>
+        <v>1.0035000000000001</v>
+      </c>
+      <c r="AA17" s="9" t="str">
+        <f t="shared" si="14"/>
+        <v>CF_L = 1.0035;</v>
+      </c>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -5077,8 +5226,19 @@
         <f t="shared" si="12"/>
         <v>CF_M = 1.0157;</v>
       </c>
-    </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y18">
+        <v>323954.875</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="13"/>
+        <v>1.0075000000000001</v>
+      </c>
+      <c r="AA18" s="9" t="str">
+        <f t="shared" si="14"/>
+        <v>CF_M = 1.0075;</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -5161,8 +5321,19 @@
         <f t="shared" si="12"/>
         <v>CF_N = 1.0592;</v>
       </c>
-    </row>
-    <row r="20" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Y19">
+        <v>1014431.75</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="13"/>
+        <v>1.0237000000000001</v>
+      </c>
+      <c r="AA19" s="9" t="str">
+        <f t="shared" si="14"/>
+        <v>CF_N = 1.0237;</v>
+      </c>
+    </row>
+    <row r="20" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -5245,8 +5416,19 @@
         <f t="shared" si="12"/>
         <v>CF_O = 1.0886;</v>
       </c>
-    </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y20">
+        <v>4190996.25</v>
+      </c>
+      <c r="Z20" s="11">
+        <f t="shared" si="13"/>
+        <v>1.1226</v>
+      </c>
+      <c r="AA20" s="9" t="str">
+        <f t="shared" si="14"/>
+        <v>CF_O = 1.1226;</v>
+      </c>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.35">
       <c r="G21" s="49" t="s">
         <v>30</v>
       </c>
@@ -5277,8 +5459,13 @@
       </c>
       <c r="W21" s="50"/>
       <c r="X21" s="51"/>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="Y21" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z21" s="50"/>
+      <c r="AA21" s="51"/>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.35">
       <c r="G22" s="13" t="s">
         <v>25</v>
       </c>
@@ -5333,8 +5520,17 @@
       <c r="X22" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Y22" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA22" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G23" s="14"/>
       <c r="H23" s="11"/>
       <c r="I23" s="12" t="e">
@@ -5378,9 +5574,27 @@
         <f>50*(W23/V23)</f>
         <v>46.416179240606724</v>
       </c>
+      <c r="Y23" s="14"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="12" t="e">
+        <f>50*(Z23/Y23)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="R28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="S29">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="Y21:AA21"/>
     <mergeCell ref="G3:R3"/>
     <mergeCell ref="B3:F4"/>
     <mergeCell ref="V4:X4"/>
@@ -5397,7 +5611,7 @@
     <mergeCell ref="G4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7451,7 +7665,7 @@
     <hyperlink ref="J27" r:id="rId6" xr:uid="{1D7CBAB8-929B-466D-89E8-0A98374378D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
   <tableParts count="1">
     <tablePart r:id="rId8"/>
   </tableParts>

</xml_diff>

<commit_message>
Working On Implementing Continuity in the Voltmeter
</commit_message>
<xml_diff>
--- a/DMM Collected Spreadsheets.xlsx
+++ b/DMM Collected Spreadsheets.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\Micro-DMM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776E5225-6953-4530-86D1-D04E29F32FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AF8DC6-2074-447B-BF8B-30A75E2364DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1850" yWindow="220" windowWidth="21430" windowHeight="14650" activeTab="1" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
+    <workbookView xWindow="2570" yWindow="370" windowWidth="21430" windowHeight="14560" activeTab="3" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Analog Circuits Reference" sheetId="2" r:id="rId1"/>
     <sheet name="Calibrations" sheetId="1" r:id="rId2"/>
     <sheet name="BOM" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="V Truth Table" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="270">
   <si>
     <t>DMM Calibration Template</t>
   </si>
@@ -828,6 +828,27 @@
   </si>
   <si>
     <t>Giga</t>
+  </si>
+  <si>
+    <t>If</t>
+  </si>
+  <si>
+    <t>Voltage Circuit Floating</t>
+  </si>
+  <si>
+    <t>Voltage Actual 0 (same net)</t>
+  </si>
+  <si>
+    <t>Voltage on Contacts</t>
+  </si>
+  <si>
+    <t>MOSFET OPEN</t>
+  </si>
+  <si>
+    <t>MOSFET CLOSED</t>
+  </si>
+  <si>
+    <t>Normal Voltmeter</t>
   </si>
 </sst>
 </file>
@@ -1087,12 +1108,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1110,6 +1125,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3840,7 +3861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CD8753-48D8-45C9-9873-856BE8983C8C}">
   <dimension ref="B2:AA29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
@@ -3859,69 +3880,69 @@
       </c>
     </row>
     <row r="3" spans="2:27" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="44" t="s">
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="44"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
     </row>
     <row r="4" spans="2:27" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="46" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="46" t="s">
+      <c r="H4" s="45"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="47"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="46" t="s">
+      <c r="K4" s="45"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="47"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="46" t="s">
+      <c r="N4" s="45"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="48"/>
-      <c r="S4" s="46" t="s">
+      <c r="Q4" s="45"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="44" t="s">
         <v>249</v>
       </c>
-      <c r="T4" s="47"/>
-      <c r="U4" s="48"/>
-      <c r="V4" s="46" t="s">
+      <c r="T4" s="45"/>
+      <c r="U4" s="46"/>
+      <c r="V4" s="44" t="s">
         <v>249</v>
       </c>
-      <c r="W4" s="47"/>
-      <c r="X4" s="48"/>
-      <c r="Y4" s="46" t="s">
+      <c r="W4" s="45"/>
+      <c r="X4" s="46"/>
+      <c r="Y4" s="44" t="s">
         <v>262</v>
       </c>
-      <c r="Z4" s="47"/>
-      <c r="AA4" s="48"/>
+      <c r="Z4" s="45"/>
+      <c r="AA4" s="46"/>
     </row>
     <row r="5" spans="2:27" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
@@ -5429,41 +5450,41 @@
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="G21" s="49" t="s">
+      <c r="G21" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="50"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="49" t="s">
+      <c r="H21" s="48"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="K21" s="50"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="49" t="s">
+      <c r="K21" s="48"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="N21" s="50"/>
-      <c r="O21" s="51"/>
-      <c r="P21" s="49" t="s">
+      <c r="N21" s="48"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="Q21" s="50"/>
-      <c r="R21" s="51"/>
-      <c r="S21" s="49" t="s">
+      <c r="Q21" s="48"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="T21" s="50"/>
-      <c r="U21" s="51"/>
-      <c r="V21" s="49" t="s">
+      <c r="T21" s="48"/>
+      <c r="U21" s="49"/>
+      <c r="V21" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="W21" s="50"/>
-      <c r="X21" s="51"/>
-      <c r="Y21" s="49" t="s">
+      <c r="W21" s="48"/>
+      <c r="X21" s="49"/>
+      <c r="Y21" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="Z21" s="50"/>
-      <c r="AA21" s="51"/>
+      <c r="Z21" s="48"/>
+      <c r="AA21" s="49"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.35">
       <c r="G22" s="13" t="s">
@@ -7674,14 +7695,51 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4371D3A1-351D-4B56-B797-13891CFDA702}">
-  <dimension ref="A1"/>
+  <dimension ref="E6:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="23.81640625" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="7" max="7" width="17.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>267</v>
+      </c>
+      <c r="G7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="8" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>266</v>
+      </c>
+      <c r="G10" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
The Giga version now can tell between floating or open in voltmeter mode
</commit_message>
<xml_diff>
--- a/DMM Collected Spreadsheets.xlsx
+++ b/DMM Collected Spreadsheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\Micro-DMM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AF8DC6-2074-447B-BF8B-30A75E2364DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E7744D-6931-481B-977F-F67A1B53A36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2570" yWindow="370" windowWidth="21430" windowHeight="14560" activeTab="3" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
+    <workbookView xWindow="330" yWindow="1940" windowWidth="21430" windowHeight="14560" activeTab="3" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Analog Circuits Reference" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="274">
   <si>
     <t>DMM Calibration Template</t>
   </si>
@@ -849,6 +849,18 @@
   </si>
   <si>
     <t>Normal Voltmeter</t>
+  </si>
+  <si>
+    <t>Voltage slams to diode limit</t>
+  </si>
+  <si>
+    <t>2.5 on both sides of bridge</t>
+  </si>
+  <si>
+    <t>0.25vdc on far ADC</t>
+  </si>
+  <si>
+    <t>2.2vdc on far ADC</t>
   </si>
 </sst>
 </file>
@@ -2326,6 +2338,229 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>641350</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D21F4E77-D915-9AE8-73D8-006DD5F73A54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2349500" y="3035300"/>
+          <a:ext cx="4146550" cy="1847850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The code looks like:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> MOSFET on</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>If: &lt;10mV on Voltage Contacts</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Then: Turn MOSFET off for  ~10mS</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> and</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> check voltage</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- If: ~2.2vdc: report "CLOSED</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>"</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- If ~.25 report "FLOAT</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>"</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>-Close</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> MOSFET, wait S seconds (2?), repeat?</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38D7DF20-7FDE-4BA9-9F8D-AB6D662DC6CF}" name="Table1" displayName="Table1" ref="A2:P36" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" dataCellStyle="Currency">
   <autoFilter ref="A2:P36" xr:uid="{38D7DF20-7FDE-4BA9-9F8D-AB6D662DC6CF}"/>
@@ -7698,14 +7933,15 @@
   <dimension ref="E6:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="5" max="5" width="23.81640625" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
-    <col min="7" max="7" width="17.36328125" customWidth="1"/>
+    <col min="6" max="6" width="25.08984375" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="5:7" x14ac:dyDescent="0.35">
@@ -7725,21 +7961,37 @@
       <c r="E8" t="s">
         <v>264</v>
       </c>
+      <c r="F8" t="s">
+        <v>272</v>
+      </c>
+      <c r="G8" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="9" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E9" t="s">
         <v>265</v>
       </c>
+      <c r="F9" t="s">
+        <v>273</v>
+      </c>
+      <c r="G9" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="10" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E10" t="s">
         <v>266</v>
       </c>
+      <c r="F10" t="s">
+        <v>270</v>
+      </c>
       <c r="G10" t="s">
         <v>269</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added feature for Giga version to report if 0vdc is due to open leads or same net.
</commit_message>
<xml_diff>
--- a/DMM Collected Spreadsheets.xlsx
+++ b/DMM Collected Spreadsheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\Micro-DMM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E7744D-6931-481B-977F-F67A1B53A36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE222437-A125-4459-A245-3F8328D4B3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="1940" windowWidth="21430" windowHeight="14560" activeTab="3" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
+    <workbookView xWindow="1360" yWindow="530" windowWidth="21430" windowHeight="14560" activeTab="3" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Analog Circuits Reference" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="277">
   <si>
     <t>DMM Calibration Template</t>
   </si>
@@ -861,6 +861,15 @@
   </si>
   <si>
     <t>2.2vdc on far ADC</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>+/- V centered about 5</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1062,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="170" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1144,6 +1153,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2912,9 +2922,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864BF7E5-8FFC-4F13-8BB7-D25F071FB544}">
-  <dimension ref="A1:T54"/>
+  <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
@@ -4037,7 +4047,7 @@
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B51" s="15">
-        <v>50</v>
+        <v>170</v>
       </c>
       <c r="C51" s="15">
         <f>C48</f>
@@ -4045,14 +4055,14 @@
       </c>
       <c r="D51" s="15">
         <f>B51*((E51+G51)/(C51+E51+G51))</f>
-        <v>26.053639846743295</v>
+        <v>86.256157635467986</v>
       </c>
       <c r="E51" s="15">
-        <v>44000</v>
+        <v>15000</v>
       </c>
       <c r="F51" s="15">
         <f>B51*((G51)/(C51+E51+G51))</f>
-        <v>23.946360153256705</v>
+        <v>83.743842364532014</v>
       </c>
       <c r="G51" s="15">
         <f>C48</f>
@@ -4073,11 +4083,34 @@
     <row r="54" spans="2:10" x14ac:dyDescent="0.35">
       <c r="G54" s="15">
         <f>D51-F51</f>
-        <v>2.1072796934865892</v>
+        <v>2.5123152709359715</v>
       </c>
       <c r="J54" s="15">
         <f>(C51+G51)/E51</f>
-        <v>22.727272727272727</v>
+        <v>66.666666666666671</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="G57" s="52" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="G59" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="G60" s="15">
+        <f>2.5-G54</f>
+        <v>-1.2315270935971512E-2</v>
+      </c>
+      <c r="H60" s="15">
+        <f>2.5+G54</f>
+        <v>5.0123152709359715</v>
       </c>
     </row>
   </sheetData>
@@ -4096,8 +4129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CD8753-48D8-45C9-9873-856BE8983C8C}">
   <dimension ref="B2:AA29"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+    <sheetView topLeftCell="N3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5830,11 +5863,15 @@
         <f>50*(W23/V23)</f>
         <v>46.416179240606724</v>
       </c>
-      <c r="Y23" s="14"/>
-      <c r="Z23" s="11"/>
-      <c r="AA23" s="12" t="e">
-        <f>50*(Z23/Y23)</f>
-        <v>#DIV/0!</v>
+      <c r="Y23" s="14">
+        <v>4.9850000000000003</v>
+      </c>
+      <c r="Z23" s="11">
+        <v>5</v>
+      </c>
+      <c r="AA23" s="12">
+        <f>67.23631*(Z23/Y23)</f>
+        <v>67.438625877632902</v>
       </c>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Minor float or closed (VAC trigger) adjustment
</commit_message>
<xml_diff>
--- a/DMM Collected Spreadsheets.xlsx
+++ b/DMM Collected Spreadsheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\Micro-DMM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE222437-A125-4459-A245-3F8328D4B3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D52655-1B9A-4594-92DB-C8A5C192D168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="530" windowWidth="21430" windowHeight="14560" activeTab="3" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="21430" windowHeight="14560" activeTab="3" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Analog Circuits Reference" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="292">
   <si>
     <t>DMM Calibration Template</t>
   </si>
@@ -830,9 +830,6 @@
     <t>Giga</t>
   </si>
   <si>
-    <t>If</t>
-  </si>
-  <si>
     <t>Voltage Circuit Floating</t>
   </si>
   <si>
@@ -870,6 +867,54 @@
   </si>
   <si>
     <t>+/- V centered about 5</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Normal Meter</t>
+  </si>
+  <si>
+    <t>Mann Voltmeter Bridge</t>
+  </si>
+  <si>
+    <t>0v</t>
+  </si>
+  <si>
+    <t>"Open Lead"</t>
+  </si>
+  <si>
+    <t>Reading is function of polarity and type</t>
+  </si>
+  <si>
+    <t>Probes Seperated By</t>
+  </si>
+  <si>
+    <t>None - Same Net</t>
+  </si>
+  <si>
+    <t>Air Gapped</t>
+  </si>
+  <si>
+    <t>Open Relay</t>
+  </si>
+  <si>
+    <t>Voltage Drop</t>
+  </si>
+  <si>
+    <t>Truth Table</t>
+  </si>
+  <si>
+    <t>Diode (unenergized)</t>
+  </si>
+  <si>
+    <t>Transfomer, primary to secondard, (unenergized)</t>
+  </si>
+  <si>
+    <t>"Undefined" - Function of Impedance</t>
+  </si>
+  <si>
+    <t>Resistor, or other impedance, energized</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1107,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="170" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1126,6 +1171,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1153,7 +1199,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2352,16 +2400,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>641350</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>882650</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2376,7 +2424,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2349500" y="3035300"/>
+          <a:off x="2590800" y="1974850"/>
           <a:ext cx="4146550" cy="1847850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2549,6 +2597,17 @@
             <a:rPr lang="en-US"/>
             <a:t> </a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>- If between those</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0"/>
+            <a:t> values report "UNDEFINED"</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
@@ -2948,14 +3007,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
       <c r="O1" s="17" t="s">
         <v>34</v>
       </c>
@@ -4091,16 +4150,16 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="G57" s="52" t="s">
-        <v>276</v>
+      <c r="G57" s="43" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.35">
       <c r="G59" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="H59" s="15" t="s">
         <v>274</v>
-      </c>
-      <c r="H59" s="15" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.35">
@@ -4148,69 +4207,69 @@
       </c>
     </row>
     <row r="3" spans="2:27" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="50" t="s">
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
     </row>
     <row r="4" spans="2:27" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="44" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="44" t="s">
+      <c r="H4" s="46"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="45"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="44" t="s">
+      <c r="K4" s="46"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="45"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="44" t="s">
+      <c r="N4" s="46"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="44" t="s">
+      <c r="Q4" s="46"/>
+      <c r="R4" s="47"/>
+      <c r="S4" s="45" t="s">
         <v>249</v>
       </c>
-      <c r="T4" s="45"/>
-      <c r="U4" s="46"/>
-      <c r="V4" s="44" t="s">
+      <c r="T4" s="46"/>
+      <c r="U4" s="47"/>
+      <c r="V4" s="45" t="s">
         <v>249</v>
       </c>
-      <c r="W4" s="45"/>
-      <c r="X4" s="46"/>
-      <c r="Y4" s="44" t="s">
+      <c r="W4" s="46"/>
+      <c r="X4" s="47"/>
+      <c r="Y4" s="45" t="s">
         <v>262</v>
       </c>
-      <c r="Z4" s="45"/>
-      <c r="AA4" s="46"/>
+      <c r="Z4" s="46"/>
+      <c r="AA4" s="47"/>
     </row>
     <row r="5" spans="2:27" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
@@ -5718,41 +5777,41 @@
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="G21" s="47" t="s">
+      <c r="G21" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="48"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="47" t="s">
+      <c r="H21" s="49"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="K21" s="48"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="47" t="s">
+      <c r="K21" s="49"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="N21" s="48"/>
-      <c r="O21" s="49"/>
-      <c r="P21" s="47" t="s">
+      <c r="N21" s="49"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="Q21" s="48"/>
-      <c r="R21" s="49"/>
-      <c r="S21" s="47" t="s">
+      <c r="Q21" s="49"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="T21" s="48"/>
-      <c r="U21" s="49"/>
-      <c r="V21" s="47" t="s">
+      <c r="T21" s="49"/>
+      <c r="U21" s="50"/>
+      <c r="V21" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="W21" s="48"/>
-      <c r="X21" s="49"/>
-      <c r="Y21" s="47" t="s">
+      <c r="W21" s="49"/>
+      <c r="X21" s="50"/>
+      <c r="Y21" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="Z21" s="48"/>
-      <c r="AA21" s="49"/>
+      <c r="Z21" s="49"/>
+      <c r="AA21" s="50"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.35">
       <c r="G22" s="13" t="s">
@@ -7967,67 +8026,159 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4371D3A1-351D-4B56-B797-13891CFDA702}">
-  <dimension ref="E6:G10"/>
+  <dimension ref="E6:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="E24" sqref="E24:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="23.81640625" customWidth="1"/>
+    <col min="5" max="5" width="29.26953125" customWidth="1"/>
     <col min="6" max="6" width="25.08984375" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
     <col min="8" max="8" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="5:7" x14ac:dyDescent="0.35">
-      <c r="E6" t="s">
-        <v>263</v>
-      </c>
+      <c r="E6" s="53" t="s">
+        <v>287</v>
+      </c>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
     </row>
     <row r="7" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>276</v>
+      </c>
       <c r="F7" t="s">
+        <v>266</v>
+      </c>
+      <c r="G7" t="s">
         <v>267</v>
-      </c>
-      <c r="G7" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="8" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G10" t="s">
-        <v>269</v>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E24" t="s">
+        <v>282</v>
+      </c>
+      <c r="F24" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="53"/>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>277</v>
+      </c>
+      <c r="G25" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E26" t="s">
+        <v>283</v>
+      </c>
+      <c r="F26" t="s">
+        <v>279</v>
+      </c>
+      <c r="G26" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E27" t="s">
+        <v>284</v>
+      </c>
+      <c r="F27" t="s">
+        <v>279</v>
+      </c>
+      <c r="G27" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E28" t="s">
+        <v>285</v>
+      </c>
+      <c r="F28" t="s">
+        <v>279</v>
+      </c>
+      <c r="G28" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E29" t="s">
+        <v>288</v>
+      </c>
+      <c r="F29" t="s">
+        <v>279</v>
+      </c>
+      <c r="G29" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E30" t="s">
+        <v>289</v>
+      </c>
+      <c r="F30" t="s">
+        <v>279</v>
+      </c>
+      <c r="G30" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E31" t="s">
+        <v>291</v>
+      </c>
+      <c r="F31" t="s">
+        <v>286</v>
+      </c>
+      <c r="G31" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="E6:G6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Giga Version Refinements, Added white paper on the auto floating probes detect voltmeter design
</commit_message>
<xml_diff>
--- a/DMM Collected Spreadsheets.xlsx
+++ b/DMM Collected Spreadsheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\Micro-DMM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D52655-1B9A-4594-92DB-C8A5C192D168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFD0F15-4865-4B64-BED7-76EDD843A566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="21430" windowHeight="14560" activeTab="3" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="21430" windowHeight="14560" activeTab="1" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Analog Circuits Reference" sheetId="2" r:id="rId1"/>
@@ -4188,8 +4188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CD8753-48D8-45C9-9873-856BE8983C8C}">
   <dimension ref="B2:AA29"/>
   <sheetViews>
-    <sheetView topLeftCell="N3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA24" sqref="AA24"/>
+    <sheetView tabSelected="1" topLeftCell="N3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA23" sqref="AA23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5923,14 +5923,26 @@
         <v>46.416179240606724</v>
       </c>
       <c r="Y23" s="14">
-        <v>4.9850000000000003</v>
+        <v>5.0149999999999997</v>
       </c>
       <c r="Z23" s="11">
         <v>5</v>
       </c>
       <c r="AA23" s="12">
-        <f>67.23631*(Z23/Y23)</f>
-        <v>67.438625877632902</v>
+        <f>68.6105*(Z23/Y23)</f>
+        <v>68.405284147557339</v>
+      </c>
+    </row>
+    <row r="26" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Y26" s="14">
+        <v>-4.9850000000000003</v>
+      </c>
+      <c r="Z26" s="11">
+        <v>-5</v>
+      </c>
+      <c r="AA26" s="12">
+        <f>68.2301*(Z26/Y26)</f>
+        <v>68.435406218655956</v>
       </c>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.35">
@@ -8028,8 +8040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4371D3A1-351D-4B56-B797-13891CFDA702}">
   <dimension ref="E6:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:G31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updates to paper following updates
</commit_message>
<xml_diff>
--- a/DMM Collected Spreadsheets.xlsx
+++ b/DMM Collected Spreadsheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\Micro-DMM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFD0F15-4865-4B64-BED7-76EDD843A566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E88493-6B3D-4C46-9541-7B63899F41DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="21430" windowHeight="14560" activeTab="1" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="21430" windowHeight="14650" activeTab="3" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Analog Circuits Reference" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="304">
   <si>
     <t>DMM Calibration Template</t>
   </si>
@@ -915,6 +915,42 @@
   </si>
   <si>
     <t>Resistor, or other impedance, energized</t>
+  </si>
+  <si>
+    <t>DIO Readings</t>
+  </si>
+  <si>
+    <t>0V</t>
+  </si>
+  <si>
+    <t>DIO Set to Gnd</t>
+  </si>
+  <si>
+    <t>DIO Set to Output</t>
+  </si>
+  <si>
+    <t>Circuit Floating</t>
+  </si>
+  <si>
+    <t>Circuit Closed</t>
+  </si>
+  <si>
+    <t>DIO in Input-Pullup Mode</t>
+  </si>
+  <si>
+    <t>MCU Voltage</t>
+  </si>
+  <si>
+    <t>DIO in Input-Pulldown Mode</t>
+  </si>
+  <si>
+    <t>DIO, Floating Input</t>
+  </si>
+  <si>
+    <t>Incorrect or Bad Wiring Connection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low or </t>
   </si>
 </sst>
 </file>
@@ -4188,7 +4224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CD8753-48D8-45C9-9873-856BE8983C8C}">
   <dimension ref="B2:AA29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="N3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AA23" sqref="AA23"/>
     </sheetView>
   </sheetViews>
@@ -8038,15 +8074,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4371D3A1-351D-4B56-B797-13891CFDA702}">
-  <dimension ref="E6:G31"/>
+  <dimension ref="E6:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="29.26953125" customWidth="1"/>
+    <col min="5" max="5" width="30.81640625" customWidth="1"/>
     <col min="6" max="6" width="25.08984375" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
     <col min="8" max="8" width="23.453125" customWidth="1"/>
@@ -8184,6 +8220,89 @@
       </c>
       <c r="G31" t="s">
         <v>286</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E35" t="s">
+        <v>292</v>
+      </c>
+      <c r="F35" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="39"/>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E36" t="s">
+        <v>276</v>
+      </c>
+      <c r="F36" t="s">
+        <v>277</v>
+      </c>
+      <c r="G36" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E37" t="s">
+        <v>302</v>
+      </c>
+      <c r="F37" t="s">
+        <v>293</v>
+      </c>
+      <c r="G37" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E38" t="s">
+        <v>294</v>
+      </c>
+      <c r="F38" t="s">
+        <v>293</v>
+      </c>
+      <c r="G38" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E39" t="s">
+        <v>295</v>
+      </c>
+      <c r="F39" t="s">
+        <v>299</v>
+      </c>
+      <c r="G39" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E40" t="s">
+        <v>298</v>
+      </c>
+      <c r="F40" t="s">
+        <v>299</v>
+      </c>
+      <c r="G40" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E41" t="s">
+        <v>300</v>
+      </c>
+      <c r="F41" t="s">
+        <v>279</v>
+      </c>
+      <c r="G41" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.35">
+      <c r="E42" t="s">
+        <v>301</v>
+      </c>
+      <c r="F42" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated RA4M1 Arduino sketch for open-lead sensing
</commit_message>
<xml_diff>
--- a/DMM Collected Spreadsheets.xlsx
+++ b/DMM Collected Spreadsheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\Micro-DMM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E88493-6B3D-4C46-9541-7B63899F41DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C523EF0-EAA5-422A-B0E0-A948883DE7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="21430" windowHeight="14650" activeTab="3" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
+    <workbookView xWindow="70" yWindow="980" windowWidth="20900" windowHeight="15070" activeTab="1" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Analog Circuits Reference" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="V Truth Table" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3019,7 +3020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864BF7E5-8FFC-4F13-8BB7-D25F071FB544}">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
@@ -4224,8 +4225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CD8753-48D8-45C9-9873-856BE8983C8C}">
   <dimension ref="B2:AA29"/>
   <sheetViews>
-    <sheetView topLeftCell="N3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA23" sqref="AA23"/>
+    <sheetView tabSelected="1" topLeftCell="N3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5949,36 +5950,36 @@
         <v>46.481538894226659</v>
       </c>
       <c r="V23" s="14">
-        <v>10.087</v>
+        <v>3.6583999999999999</v>
       </c>
       <c r="W23" s="11">
-        <v>9.3640000000000008</v>
+        <v>5</v>
       </c>
       <c r="X23" s="12">
-        <f>50*(W23/V23)</f>
-        <v>46.416179240606724</v>
+        <f>50.0662*(W23/V23)</f>
+        <v>68.426361250820037</v>
       </c>
       <c r="Y23" s="14">
-        <v>5.0149999999999997</v>
+        <v>4.9950000000000001</v>
       </c>
       <c r="Z23" s="11">
         <v>5</v>
       </c>
       <c r="AA23" s="12">
-        <f>68.6105*(Z23/Y23)</f>
-        <v>68.405284147557339</v>
+        <f>68.40528*(Z23/Y23)</f>
+        <v>68.473753753753769</v>
       </c>
     </row>
     <row r="26" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="Y26" s="14">
-        <v>-4.9850000000000003</v>
+        <v>-4.9939999999999998</v>
       </c>
       <c r="Z26" s="11">
         <v>-5</v>
       </c>
       <c r="AA26" s="12">
-        <f>68.2301*(Z26/Y26)</f>
-        <v>68.435406218655956</v>
+        <f>68.43541*(Z26/Y26)</f>
+        <v>68.517631157388877</v>
       </c>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.35">
@@ -7997,7 +7998,7 @@
         <v>50</v>
       </c>
       <c r="M55" s="31">
-        <f t="shared" ref="M55" si="3">SUM(M48:M53)</f>
+        <f>SUM(M48:M53)</f>
         <v>29.834666666666664</v>
       </c>
     </row>
@@ -8076,7 +8077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4371D3A1-351D-4B56-B797-13891CFDA702}">
   <dimension ref="E6:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Working on PCBs and Separating Out Different Versions
</commit_message>
<xml_diff>
--- a/DMM Collected Spreadsheets.xlsx
+++ b/DMM Collected Spreadsheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\Micro-DMM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D3A748A-C7B4-4224-8573-8E04BA1AC76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5BFFAF-2EE6-4C95-921D-F78BEFD67027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="0" windowWidth="21660" windowHeight="15370" activeTab="1" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
+    <workbookView xWindow="630" yWindow="240" windowWidth="19960" windowHeight="14840" activeTab="1" xr2:uid="{AA7D1287-CC71-449A-9503-E2DCBFCF1F8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Analog Circuits Reference" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="V Truth Table" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4226,7 +4225,7 @@
   <dimension ref="B2:AA29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA27" sqref="AA27"/>
+      <selection activeCell="AA26" sqref="AA26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5960,26 +5959,26 @@
         <v>68.426361250820037</v>
       </c>
       <c r="Y23" s="14">
-        <v>4.9850000000000003</v>
+        <v>5.0030000000000001</v>
       </c>
       <c r="Z23" s="11">
         <v>5</v>
       </c>
       <c r="AA23" s="12">
-        <f>68.36437*(Z23/Y23)</f>
-        <v>68.570080240722163</v>
+        <f>68.57008*(Z23/Y23)</f>
+        <v>68.528962622426548</v>
       </c>
     </row>
     <row r="26" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="Y26" s="14">
-        <v>-4.9850000000000003</v>
+        <v>-4.992</v>
       </c>
       <c r="Z26" s="11">
         <v>-5</v>
       </c>
       <c r="AA26" s="12">
-        <f>68.3536*(Z26/Y26)</f>
-        <v>68.559277833500502</v>
+        <f>68.55928*(Z26/Y26)</f>
+        <v>68.669150641025638</v>
       </c>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.35">

</xml_diff>